<commit_message>
fix: add missing login_user() call to enable user session
Fixed login route by adding missing login_user() call

Ensures user session is created upon successful login

Prevents redirect loop and "Please log in" message

Verified against hashed credentials (RM / Rm1001)
</commit_message>
<xml_diff>
--- a/data/orders_2025.xlsx
+++ b/data/orders_2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masuryk\Documents\Workflow\Orders_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd3e130a03c534da/DEV/Pet_projects/Logistic_tracker/supply_tracker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EF8B1D-1735-4592-9BA7-AA9608E02D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{25EF8B1D-1735-4592-9BA7-AA9608E02D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{620222F1-1C26-4A11-AE81-8E65BE779D83}"/>
   <bookViews>
-    <workbookView xWindow="34380" yWindow="0" windowWidth="23280" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1229,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>